<commit_message>
Clear code Area Fontend
</commit_message>
<xml_diff>
--- a/TeduShop.WebAPI/Templates/OrderTemplate.xlsx
+++ b/TeduShop.WebAPI/Templates/OrderTemplate.xlsx
@@ -1,27 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\tedushop-webapi\TeduShop.WebAPI\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Visual studio 2017 project\CozaStore_WebAPI_Angular8\TeduShop.WebAPI\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121816A1-B220-4CAA-B341-9EC33E5AA01B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEDUOrder" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="0"/>
+  <calcPr calcId="191029" iterateDelta="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>HÓA ĐƠN BÁN HÀNG</t>
   </si>
@@ -61,9 +69,6 @@
   <si>
     <t>Địa chỉ: Xuân La Tây Hồ Hà Nội
 ĐT: 0966 036 626</t>
-  </si>
-  <si>
-    <t>Mặt hàng bán (Thời trang nam)</t>
   </si>
   <si>
     <t>Điện thoại:</t>
@@ -75,7 +80,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
@@ -253,12 +258,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -273,21 +293,6 @@
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -315,39 +320,39 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>809625</xdr:colOff>
+      <xdr:colOff>434612</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>266700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1619251</xdr:colOff>
+      <xdr:colOff>1895257</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>828676</xdr:rowOff>
+      <xdr:rowOff>601930</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F138D3B-3A7C-4C03-9DA4-AD21CD543054}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1181100" y="19050"/>
-          <a:ext cx="809626" cy="809626"/>
+          <a:off x="815612" y="266700"/>
+          <a:ext cx="1460645" cy="335230"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -621,76 +626,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+    <row r="1" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="29"/>
+    </row>
+    <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="29"/>
-    </row>
-    <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-    </row>
-    <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-    </row>
-    <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
-        <v>14</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -707,7 +710,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>1</v>
       </c>
@@ -719,7 +722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>2</v>
       </c>
@@ -731,7 +734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>3</v>
       </c>
@@ -743,7 +746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>4</v>
       </c>
@@ -755,7 +758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>5</v>
       </c>
@@ -767,7 +770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>6</v>
       </c>
@@ -779,7 +782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>7</v>
       </c>
@@ -791,7 +794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>8</v>
       </c>
@@ -803,7 +806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>9</v>
       </c>
@@ -815,7 +818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>10</v>
       </c>
@@ -827,7 +830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>11</v>
       </c>
@@ -839,7 +842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>12</v>
       </c>
@@ -851,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>13</v>
       </c>
@@ -863,7 +866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>14</v>
       </c>
@@ -875,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>15</v>
       </c>
@@ -887,11 +890,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="24" t="s">
+    <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="24"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="3">
         <f>SUM(C9:C23)</f>
         <v>0</v>
@@ -902,38 +905,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="25"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C28" s="26" t="s">
+    <row r="26" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="s">
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="28" t="s">
+      <c r="B29" s="22"/>
+      <c r="C29" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:E29"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:E1"/>
@@ -941,6 +939,11 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:E29"/>
   </mergeCells>
   <pageMargins left="0.55069444444444449" right="0.2361111111111111" top="0.47222222222222221" bottom="0.35416666666666669" header="0.31458333333333333" footer="0.27500000000000002"/>
   <pageSetup paperSize="9" firstPageNumber="4294963191" orientation="portrait" r:id="rId1"/>
@@ -950,12 +953,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="4294963191" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -964,12 +967,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="4294963191" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>